<commit_message>
fix: Manifest MD5s, Excel named ranges, and documentation gaps
</commit_message>
<xml_diff>
--- a/06_Exports/clv_inputs_v1.1.xlsx
+++ b/06_Exports/clv_inputs_v1.1.xlsx
@@ -10,17 +10,23 @@
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Monthly_Data" sheetId="2" r:id="rId2"/>
     <sheet name="User_Summary" sheetId="3" r:id="rId3"/>
+    <sheet name="README" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Discount_Rate">Inputs!$B$3</definedName>
-    <definedName name="Gross_Margin">Inputs!$B$2</definedName>
+    <definedName name="cac_target">Inputs!$B$8</definedName>
+    <definedName name="discount_rate">Inputs!$B$3</definedName>
+    <definedName name="gross_margin">Inputs!$B$2</definedName>
+    <definedName name="monthly_churn_basic">Inputs!$B$6</definedName>
+    <definedName name="monthly_churn_pro">Inputs!$B$7</definedName>
+    <definedName name="price_basic">Inputs!$B$4</definedName>
+    <definedName name="price_pro">Inputs!$B$5</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Parameter</t>
   </si>
@@ -28,6 +34,9 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Key</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -37,25 +46,55 @@
     <t>Discount Rate</t>
   </si>
   <si>
-    <t>Basic Price</t>
-  </si>
-  <si>
-    <t>Pro Price</t>
+    <t>Price Basic</t>
+  </si>
+  <si>
+    <t>Price Pro</t>
+  </si>
+  <si>
+    <t>Monthly Churn Basic</t>
+  </si>
+  <si>
+    <t>Monthly Churn Pro</t>
   </si>
   <si>
     <t>CAC Target</t>
   </si>
   <si>
+    <t>gross_margin</t>
+  </si>
+  <si>
+    <t>discount_rate</t>
+  </si>
+  <si>
+    <t>price_basic</t>
+  </si>
+  <si>
+    <t>price_pro</t>
+  </si>
+  <si>
+    <t>monthly_churn_basic</t>
+  </si>
+  <si>
+    <t>monthly_churn_pro</t>
+  </si>
+  <si>
+    <t>cac_target</t>
+  </si>
+  <si>
     <t>Margin after COGS</t>
   </si>
   <si>
     <t>Annual WACC</t>
   </si>
   <si>
-    <t>Monthly Basic</t>
-  </si>
-  <si>
-    <t>Monthly Pro</t>
+    <t>Monthly Basic Price</t>
+  </si>
+  <si>
+    <t>Monthly Pro Price</t>
+  </si>
+  <si>
+    <t>Est. Monthly Churn</t>
   </si>
   <si>
     <t>Target Cost per Acq</t>
@@ -131,6 +170,15 @@
   </si>
   <si>
     <t>Avg_Retention</t>
+  </si>
+  <si>
+    <t>This file contains inputs for the CLV model.</t>
+  </si>
+  <si>
+    <t>Do not rename sheets.</t>
+  </si>
+  <si>
+    <t>Named Ranges defined: gross_margin, discount_rate, price_basic, price_pro, etc.</t>
   </si>
 </sst>
 </file>
@@ -488,13 +536,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,60 +552,106 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>0.85</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.1</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6">
+        <v>0.05</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.02</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
         <v>150</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -575,39 +669,39 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>15560</v>
@@ -639,7 +733,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>47515</v>
@@ -671,7 +765,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>78911</v>
@@ -703,7 +797,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>106866</v>
@@ -735,7 +829,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>130289</v>
@@ -767,7 +861,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>151826</v>
@@ -799,7 +893,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>170154</v>
@@ -831,7 +925,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>191993</v>
@@ -863,7 +957,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>216478</v>
@@ -895,7 +989,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>248326</v>
@@ -927,7 +1021,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>282910</v>
@@ -959,7 +1053,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>311809</v>
@@ -1004,10 +1098,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1104,6 +1198,34 @@
       </c>
       <c r="B13">
         <v>0.1621900826446281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Final cleanup - manifest, duplicate files, and Excel names
</commit_message>
<xml_diff>
--- a/06_Exports/clv_inputs_v1.1.xlsx
+++ b/06_Exports/clv_inputs_v1.1.xlsx
@@ -11,9 +11,12 @@
     <sheet name="Monthly_Data" sheetId="2" r:id="rId2"/>
     <sheet name="User_Summary" sheetId="3" r:id="rId3"/>
     <sheet name="README" sheetId="4" r:id="rId4"/>
+    <sheet name="__names__" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="activation_rate">Inputs!$B$9</definedName>
     <definedName name="cac_target">Inputs!$B$8</definedName>
+    <definedName name="conversion_rate">Inputs!$B$10</definedName>
     <definedName name="discount_rate">Inputs!$B$3</definedName>
     <definedName name="gross_margin">Inputs!$B$2</definedName>
     <definedName name="monthly_churn_basic">Inputs!$B$6</definedName>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="69">
   <si>
     <t>Parameter</t>
   </si>
@@ -61,6 +64,12 @@
     <t>CAC Target</t>
   </si>
   <si>
+    <t>Activation Rate</t>
+  </si>
+  <si>
+    <t>Conversion Rate</t>
+  </si>
+  <si>
     <t>gross_margin</t>
   </si>
   <si>
@@ -82,6 +91,12 @@
     <t>cac_target</t>
   </si>
   <si>
+    <t>activation_rate</t>
+  </si>
+  <si>
+    <t>conversion_rate</t>
+  </si>
+  <si>
     <t>Margin after COGS</t>
   </si>
   <si>
@@ -94,12 +109,21 @@
     <t>Monthly Pro Price</t>
   </si>
   <si>
-    <t>Est. Monthly Churn</t>
+    <t>Est. Monthly Churn B</t>
+  </si>
+  <si>
+    <t>Est. Monthly Churn P</t>
   </si>
   <si>
     <t>Target Cost per Acq</t>
   </si>
   <si>
+    <t>Est. Activation %</t>
+  </si>
+  <si>
+    <t>Est. Trial-to-Paid %</t>
+  </si>
+  <si>
     <t>month</t>
   </si>
   <si>
@@ -179,6 +203,39 @@
   </si>
   <si>
     <t>Named Ranges defined: gross_margin, discount_rate, price_basic, price_pro, etc.</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>RefersTo</t>
+  </si>
+  <si>
+    <t>Inputs!$B$2</t>
+  </si>
+  <si>
+    <t>Inputs!$B$3</t>
+  </si>
+  <si>
+    <t>Inputs!$B$4</t>
+  </si>
+  <si>
+    <t>Inputs!$B$5</t>
+  </si>
+  <si>
+    <t>Inputs!$B$6</t>
+  </si>
+  <si>
+    <t>Inputs!$B$7</t>
+  </si>
+  <si>
+    <t>Inputs!$B$8</t>
+  </si>
+  <si>
+    <t>Inputs!$B$9</t>
+  </si>
+  <si>
+    <t>Inputs!$B$10</t>
   </si>
 </sst>
 </file>
@@ -536,7 +593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -564,10 +621,10 @@
         <v>0.85</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -578,10 +635,10 @@
         <v>0.1</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -592,10 +649,10 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -606,10 +663,10 @@
         <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -620,10 +677,10 @@
         <v>0.05</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -634,10 +691,10 @@
         <v>0.02</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -648,10 +705,38 @@
         <v>150</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>0.3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>0.05</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -669,39 +754,39 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>15560</v>
@@ -733,7 +818,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>47515</v>
@@ -765,7 +850,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>78911</v>
@@ -797,7 +882,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <v>106866</v>
@@ -829,7 +914,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>130289</v>
@@ -861,7 +946,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>151826</v>
@@ -893,7 +978,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>170154</v>
@@ -925,7 +1010,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>191993</v>
@@ -957,7 +1042,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>216478</v>
@@ -989,7 +1074,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>248326</v>
@@ -1021,7 +1106,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B12">
         <v>282910</v>
@@ -1053,7 +1138,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B13">
         <v>311809</v>
@@ -1098,10 +1183,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1215,17 +1300,110 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: MRR bridge inclusive end-date logic (Diff 256.0 resolved)
</commit_message>
<xml_diff>
--- a/06_Exports/clv_inputs_v1.1.xlsx
+++ b/06_Exports/clv_inputs_v1.1.xlsx
@@ -821,7 +821,7 @@
         <v>42</v>
       </c>
       <c r="B3">
-        <v>47515</v>
+        <v>47841</v>
       </c>
       <c r="C3">
         <v>15560</v>
@@ -836,13 +836,13 @@
         <v>-0</v>
       </c>
       <c r="G3">
-        <v>1263</v>
+        <v>937</v>
       </c>
       <c r="H3">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="I3">
-        <v>199.6428571428572</v>
+        <v>197.6900826446281</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -853,13 +853,13 @@
         <v>43</v>
       </c>
       <c r="B4">
-        <v>78911</v>
+        <v>79097</v>
       </c>
       <c r="C4">
-        <v>47515</v>
+        <v>47841</v>
       </c>
       <c r="D4">
-        <v>32164</v>
+        <v>32024</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -871,10 +871,10 @@
         <v>768</v>
       </c>
       <c r="H4">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="I4">
-        <v>203.9043927648579</v>
+        <v>202.2941176470588</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -885,13 +885,13 @@
         <v>44</v>
       </c>
       <c r="B5">
-        <v>106866</v>
+        <v>107093</v>
       </c>
       <c r="C5">
-        <v>78911</v>
+        <v>79097</v>
       </c>
       <c r="D5">
-        <v>29177</v>
+        <v>28991</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -900,13 +900,13 @@
         <v>-0</v>
       </c>
       <c r="G5">
-        <v>1222</v>
+        <v>995</v>
       </c>
       <c r="H5">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="I5">
-        <v>201.2542372881356</v>
+        <v>200.5486891385768</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -917,13 +917,13 @@
         <v>45</v>
       </c>
       <c r="B6">
-        <v>130289</v>
+        <v>130516</v>
       </c>
       <c r="C6">
-        <v>106866</v>
+        <v>107093</v>
       </c>
       <c r="D6">
-        <v>24459</v>
+        <v>24488</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -932,13 +932,13 @@
         <v>-0</v>
       </c>
       <c r="G6">
-        <v>1036</v>
+        <v>1065</v>
       </c>
       <c r="H6">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="I6">
-        <v>206.1534810126582</v>
+        <v>205.5370078740158</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -949,13 +949,13 @@
         <v>46</v>
       </c>
       <c r="B7">
-        <v>151826</v>
+        <v>151855</v>
       </c>
       <c r="C7">
-        <v>130289</v>
+        <v>130516</v>
       </c>
       <c r="D7">
-        <v>22107</v>
+        <v>21880</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -964,13 +964,13 @@
         <v>-0</v>
       </c>
       <c r="G7">
-        <v>570</v>
+        <v>541</v>
       </c>
       <c r="H7">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="I7">
-        <v>203.793288590604</v>
+        <v>203.558981233244</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -981,13 +981,13 @@
         <v>47</v>
       </c>
       <c r="B8">
-        <v>170154</v>
+        <v>170282</v>
       </c>
       <c r="C8">
-        <v>151826</v>
+        <v>151855</v>
       </c>
       <c r="D8">
-        <v>19014</v>
+        <v>19113</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -999,10 +999,10 @@
         <v>686</v>
       </c>
       <c r="H8">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="I8">
-        <v>205.2521109770808</v>
+        <v>204.9121540312876</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1013,13 +1013,13 @@
         <v>48</v>
       </c>
       <c r="B9">
-        <v>191993</v>
+        <v>192220</v>
       </c>
       <c r="C9">
-        <v>170154</v>
+        <v>170282</v>
       </c>
       <c r="D9">
-        <v>22450</v>
+        <v>22578</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1028,13 +1028,13 @@
         <v>-0</v>
       </c>
       <c r="G9">
-        <v>611</v>
+        <v>640</v>
       </c>
       <c r="H9">
-        <v>948</v>
+        <v>951</v>
       </c>
       <c r="I9">
-        <v>202.5242616033755</v>
+        <v>202.124079915878</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1045,13 +1045,13 @@
         <v>49</v>
       </c>
       <c r="B10">
-        <v>216478</v>
+        <v>216536</v>
       </c>
       <c r="C10">
-        <v>191993</v>
+        <v>192220</v>
       </c>
       <c r="D10">
-        <v>25113</v>
+        <v>24886</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1060,13 +1060,13 @@
         <v>-0</v>
       </c>
       <c r="G10">
-        <v>628</v>
+        <v>570</v>
       </c>
       <c r="H10">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="I10">
-        <v>200.2571692876966</v>
+        <v>199.9409048938135</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1077,13 +1077,13 @@
         <v>50</v>
       </c>
       <c r="B11">
-        <v>248326</v>
+        <v>248355</v>
       </c>
       <c r="C11">
-        <v>216478</v>
+        <v>216536</v>
       </c>
       <c r="D11">
-        <v>32674</v>
+        <v>32645</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1095,10 +1095,10 @@
         <v>826</v>
       </c>
       <c r="H11">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="I11">
-        <v>203.3791973791974</v>
+        <v>203.2364975450081</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1109,13 +1109,13 @@
         <v>51</v>
       </c>
       <c r="B12">
-        <v>282910</v>
+        <v>282968</v>
       </c>
       <c r="C12">
-        <v>248326</v>
+        <v>248355</v>
       </c>
       <c r="D12">
-        <v>36219</v>
+        <v>36190</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1124,13 +1124,13 @@
         <v>-0</v>
       </c>
       <c r="G12">
-        <v>1635</v>
+        <v>1577</v>
       </c>
       <c r="H12">
-        <v>1366</v>
+        <v>1368</v>
       </c>
       <c r="I12">
-        <v>207.1083455344071</v>
+        <v>206.8479532163742</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1141,13 +1141,13 @@
         <v>52</v>
       </c>
       <c r="B13">
-        <v>311809</v>
+        <v>312065</v>
       </c>
       <c r="C13">
-        <v>282910</v>
+        <v>282968</v>
       </c>
       <c r="D13">
-        <v>30085</v>
+        <v>30312</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1156,13 +1156,13 @@
         <v>-0</v>
       </c>
       <c r="G13">
-        <v>1186</v>
+        <v>1215</v>
       </c>
       <c r="H13">
-        <v>1484</v>
+        <v>1488</v>
       </c>
       <c r="I13">
-        <v>210.1138814016172</v>
+        <v>209.7211021505376</v>
       </c>
       <c r="J13">
         <v>0</v>

</xml_diff>